<commit_message>
switch caps for lower cost
</commit_message>
<xml_diff>
--- a/BOM/BOM.xlsx
+++ b/BOM/BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ravi\Git\esp32-devboard\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{E953F376-461A-497E-BFA6-A26E47E6DAA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF31C5C6-C484-4884-AC6D-05257AF39B07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="19543" windowHeight="12377" xr2:uid="{5E4FC15B-0B20-4E29-A061-84101F7C94AB}"/>
   </bookViews>
@@ -49,9 +49,6 @@
     <t>0.1u</t>
   </si>
   <si>
-    <t>C0603G104K5RACT250</t>
-  </si>
-  <si>
     <t>C8</t>
   </si>
   <si>
@@ -170,6 +167,9 @@
   </si>
   <si>
     <t>AMS1117-3.3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UMK107B7104KAHT </t>
   </si>
 </sst>
 </file>
@@ -1033,7 +1033,7 @@
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="D2" sqref="D2:D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1082,124 +1082,124 @@
         <v>7</v>
       </c>
       <c r="D3" t="s">
-        <v>9</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
         <v>10</v>
-      </c>
-      <c r="B4" t="s">
-        <v>11</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
         <v>13</v>
-      </c>
-      <c r="B5" t="s">
-        <v>14</v>
       </c>
       <c r="C5">
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" t="s">
         <v>15</v>
-      </c>
-      <c r="B6" t="s">
-        <v>16</v>
       </c>
       <c r="C6">
         <v>3</v>
       </c>
       <c r="D6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" t="s">
         <v>18</v>
-      </c>
-      <c r="B7" t="s">
-        <v>19</v>
       </c>
       <c r="C7">
         <v>3</v>
       </c>
       <c r="D7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" t="s">
         <v>21</v>
-      </c>
-      <c r="B8" t="s">
-        <v>22</v>
       </c>
       <c r="C8">
         <v>1</v>
       </c>
       <c r="D8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" t="s">
         <v>24</v>
-      </c>
-      <c r="B9" t="s">
-        <v>25</v>
       </c>
       <c r="C9">
         <v>1</v>
       </c>
       <c r="D9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" t="s">
         <v>27</v>
-      </c>
-      <c r="B10" t="s">
-        <v>28</v>
       </c>
       <c r="C10">
         <v>1</v>
       </c>
       <c r="D10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" t="s">
         <v>30</v>
-      </c>
-      <c r="B11" t="s">
-        <v>31</v>
       </c>
       <c r="C11">
         <v>2</v>
       </c>
       <c r="D11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B12">
         <v>47</v>
@@ -1208,71 +1208,71 @@
         <v>3</v>
       </c>
       <c r="D12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13" t="s">
         <v>35</v>
-      </c>
-      <c r="B13" t="s">
-        <v>36</v>
       </c>
       <c r="C13">
         <v>3</v>
       </c>
       <c r="D13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
+        <v>37</v>
+      </c>
+      <c r="B14" t="s">
         <v>38</v>
-      </c>
-      <c r="B14" t="s">
-        <v>39</v>
       </c>
       <c r="C14">
         <v>1</v>
       </c>
       <c r="D14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C15">
         <v>1</v>
       </c>
       <c r="D15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B16" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C16">
         <v>4</v>
       </c>
       <c r="D16" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C17">
         <v>2</v>
@@ -1280,30 +1280,30 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
+        <v>45</v>
+      </c>
+      <c r="B18" t="s">
         <v>46</v>
-      </c>
-      <c r="B18" t="s">
-        <v>47</v>
       </c>
       <c r="C18">
         <v>1</v>
       </c>
       <c r="D18" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
+        <v>47</v>
+      </c>
+      <c r="B19" t="s">
         <v>48</v>
-      </c>
-      <c r="B19" t="s">
-        <v>49</v>
       </c>
       <c r="C19">
         <v>1</v>
       </c>
       <c r="D19" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>